<commit_message>
Cambios modelos con colisiones y musica
Agregué una música para el juego cute y los modelos cuentan con colliders
</commit_message>
<xml_diff>
--- a/Documentos/PosicionesObjetos.xlsx
+++ b/Documentos/PosicionesObjetos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diana\OneDrive\Documentos\() UNAMCOMPUTACION\11vo\Computación Grafica Avanzada\Proyecto2\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713BBAC7-24E0-47C0-92ED-55F08967B675}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB65D53E-A73C-4F9B-ACBA-697C653FDDBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4452" yWindow="0" windowWidth="12552" windowHeight="12360" xr2:uid="{2087185A-5EFE-4DDD-AE7D-767E05F9C834}"/>
+    <workbookView xWindow="9324" yWindow="0" windowWidth="12552" windowHeight="12360" xr2:uid="{2087185A-5EFE-4DDD-AE7D-767E05F9C834}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -114,7 +114,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +124,21 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -161,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -177,6 +192,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89243601-6424-426B-A9E9-401D3AA38A7E}">
   <dimension ref="A1:F139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D108" sqref="D108"/>
+    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1861,7 +1882,7 @@
       <c r="B67" s="2">
         <v>453</v>
       </c>
-      <c r="C67" s="2">
+      <c r="C67" s="8">
         <v>183</v>
       </c>
       <c r="D67" s="2">
@@ -2001,11 +2022,11 @@
       <c r="C73" s="2">
         <v>656</v>
       </c>
-      <c r="D73" s="2">
+      <c r="D73" s="7">
         <f t="shared" si="2"/>
         <v>-412.5</v>
       </c>
-      <c r="E73" s="2">
+      <c r="E73" s="7">
         <f t="shared" si="3"/>
         <v>-351.5625</v>
       </c>

</xml_diff>